<commit_message>
update gauge flow data extraction
</commit_message>
<xml_diff>
--- a/preprocessing/USGS Gauge Flow Data extraction/USGS gauges.xlsx
+++ b/preprocessing/USGS Gauge Flow Data extraction/USGS gauges.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\PROJECTS\SIERRA2\Pywr models\preprocessing\USGS Gauge Flow Data extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477558CF-D9DC-4B74-83F2-C7FD64442911}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF78EE7F-4CCC-4515-AE01-DE84D47E67C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="merced-streamflow" sheetId="1" r:id="rId1"/>
-    <sheet name="merced-storage" sheetId="3" r:id="rId2"/>
+    <sheet name="merced - streamflow" sheetId="1" r:id="rId1"/>
+    <sheet name="merced - storage" sheetId="3" r:id="rId2"/>
     <sheet name="stanislaus" sheetId="2" r:id="rId3"/>
+    <sheet name="upper san joaquin - streamflow" sheetId="4" r:id="rId4"/>
+    <sheet name="upper san joaquin - storage" sheetId="5" r:id="rId5"/>
+    <sheet name="tuolumne - streamflow" sheetId="6" r:id="rId6"/>
+    <sheet name="tuolumne - storage" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>USGS 11264500 MERCED R A HAPPY ISLES BRIDGE NR YOSEMITE CA</t>
   </si>
@@ -159,6 +163,228 @@
   </si>
   <si>
     <t>USGS 11269700 EXCHEQUER PH A EXCHEQUER CA</t>
+  </si>
+  <si>
+    <t>USGS 11226500 SAN JOAQUIN R A MILLER CROSSING CA</t>
+  </si>
+  <si>
+    <t>USGS 11229500 WARD TUNNEL A INTAKE A FLORENCE LAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11230070 SF SAN JOAQUIN R AB HOOPER C NR FLORENCE LAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11230215 SF SAN JOAQUIN R BL HOOPER C NR FLORENCE LAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11230500 BEAR C NR LAKE THOMAS A EDISON CA</t>
+  </si>
+  <si>
+    <t>USGS 11230520 BEAR C CONDUIT NR LAKE THOMAS A EDISON CA</t>
+  </si>
+  <si>
+    <t>USGS 11230530 BEAR C BELOW DIV DAM NR LAKE THOMAS A EDISON CA</t>
+  </si>
+  <si>
+    <t>USGS 11230560 CHINQUAPIN C BL DIV DAM NR BIG C CA</t>
+  </si>
+  <si>
+    <t>USGS 11230600 CAMP 62 C BL DIV DAM NR BIG C CA</t>
+  </si>
+  <si>
+    <t>USGS 11230670 BOLSILLO C BL DIV DAM NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11231500 MONO C BL LK THOMAS A EDISON CA</t>
+  </si>
+  <si>
+    <t>USGS 11231550 MONO C CONDUIT NR MONO HOT SPRINGS CA</t>
+  </si>
+  <si>
+    <t>USGS 11231600 MONO C BL DIV DAM NR MONO HOT SPRINGS CA</t>
+  </si>
+  <si>
+    <t>USGS 11234760 SAN JOAQUIN R AB SHAKEFLAT C NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11235100 MAMMOTH POOL PP NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11235500 PORTAL POWERPLANT AT HUNTINGTON LAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11237000 BIG C BL HUNTINGTON LK CA</t>
+  </si>
+  <si>
+    <t>USGS 11237500 PITMAN C BL TAMARACK C CA</t>
+  </si>
+  <si>
+    <t>USGS 11237700 PITMAN C NR TAMARACK MOUNTAIN CA</t>
+  </si>
+  <si>
+    <t>USGS 11238100 BIG C PH NO 1 AT BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11238250 EASTWOOD PP AB SHAVER LK NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11238270 MF BALSAM C BL BALSAM MDW FOREBAY NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11238380 BIG C PH NO 2 NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11238400 BIG C PH NO 2A NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11238500 BIG C NR MOUTH NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11238550 BIG C PH NO 8 NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11239300 NF STEVENSON C A PERIMETER RD NR BIG C CA</t>
+  </si>
+  <si>
+    <t>USGS 11241500 STEVENSON C A SHAVER LK CA</t>
+  </si>
+  <si>
+    <t>USGS 11241800 BIG C PH NO 3 NR SHAVER LK CA</t>
+  </si>
+  <si>
+    <t>USGS 11242000 SAN JOAQUIN R AB WILLOW C NR AUBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11242400 NF WILLOW C NR SUGAR PINE CA</t>
+  </si>
+  <si>
+    <t>USGS 11243300 BROWNS C CN AT BASS LAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11243500 PGE NO 3 CONDUIT NR BASS LAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11244000 NF WILLOW C NR BASS LAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11244100 SAN JOAQUIN PH NO3 NR NORTH FORK CA</t>
+  </si>
+  <si>
+    <t>USGS 11246500 WILLOW C A MOUTH NR AUBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11246530 BIG C PH NO 4 NR AUBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11246570 SAN JOAQUIN PH NO2 NR NORTH FORK CA</t>
+  </si>
+  <si>
+    <t>USGS 11246590 SAN JOAQUIN PH NO1A NR AUBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11246610 SAN JOAQUIN PH NO1 NR AUBERRY (WISHON PH) CA</t>
+  </si>
+  <si>
+    <t>USGS 11246700 SAN JOAQUIN R NR AUBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11246950 KERCKHOFF PH NR AUBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11247050 KERCKHOFF PH NO 2 A MILLERTON LK NR AUBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11229600 FLORENCE LK NR BIG C CA</t>
+  </si>
+  <si>
+    <t>USGS 11236000 HUNTINGTON LK NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11243400 BASS LK NR BASS LAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11234700 MAMMOTH POOL RE NR BIG CREEK CA</t>
+  </si>
+  <si>
+    <t>USGS 11231000 LK THOMAS A. EDISON NR BIG C CA</t>
+  </si>
+  <si>
+    <t>USGS 11246650 KERCKHOFF RES NR AUBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11250100 MILLERTON LK A FRIANT CA</t>
+  </si>
+  <si>
+    <t>USGS 11241950 REDINGER LK NR AUBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11239500 SHAVER LK NR BIG C CA</t>
+  </si>
+  <si>
+    <t>USGS 11276500 TUOLUMNE R NR HETCH HETCHY CA</t>
+  </si>
+  <si>
+    <t>USGS 11276600 TUOLUMNE R AB EARLY INTAKE NR MATHER CA</t>
+  </si>
+  <si>
+    <t>USGS 11276900 TUOLUMNE R BL EARLY INTAKE NR MATHER CA</t>
+  </si>
+  <si>
+    <t>USGS 11277300 CHERRY C BL VALLEY DAM NR HETCH HETCHY CA</t>
+  </si>
+  <si>
+    <t>USGS 11278000 ELEANOR C NR HETCH HETCHY CA</t>
+  </si>
+  <si>
+    <t>USGS 11278200 CHERRY C CN NR EARLY INTAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11278300 CHERRY C NR EARLY INTAKE CA</t>
+  </si>
+  <si>
+    <t>USGS 11278400 CHERRY C BL DION R HOLM PH NR MATHER CA</t>
+  </si>
+  <si>
+    <t>USGS 11281000 SF TUOLUMNE R NR OAKLAND RECREATION CAMP CA</t>
+  </si>
+  <si>
+    <t>USGS 11282000 M TUOLUMNE R A OAKLAND RECREATION CAMP CA</t>
+  </si>
+  <si>
+    <t>USGS 11283250 CLAVEY R NR LONG BARN CA</t>
+  </si>
+  <si>
+    <t>USGS 11283350 REED C NR LONG BARN CA</t>
+  </si>
+  <si>
+    <t>USGS 11283500 CLAVEY R NR BUCK MEADOWS CA</t>
+  </si>
+  <si>
+    <t>USGS 11284400 BIG C AB WHITES GULCH NR GROVELAND CA</t>
+  </si>
+  <si>
+    <t>USGS 11284700 NF TUOLUMNE R NR LONG BARN CA</t>
+  </si>
+  <si>
+    <t>USGS 11275500 HETCH HETCHY RES A HETCH HETCHY CA</t>
+  </si>
+  <si>
+    <t>USGS 11277500 LK ELEANOR NR HETCH HETCHY CA</t>
+  </si>
+  <si>
+    <t>USGS 11277200 CHERRY LK NR HETCH HETCHY CA</t>
+  </si>
+  <si>
+    <t>USGS 11287500 DON PEDRO RES NR LA GRANGE CA</t>
+  </si>
+  <si>
+    <t>USGS 11289000 MODESTO CN NR LA GRANGE CA</t>
+  </si>
+  <si>
+    <t>USGS 11289500 TURLOCK CN NR LA GRANGE CA</t>
+  </si>
+  <si>
+    <t>USGS 11289650 TUOLUMNE R BL LAGRANGE DAM NR LAGRANGE CA</t>
   </si>
 </sst>
 </file>
@@ -478,42 +704,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.61328125" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -528,20 +754,20 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -560,187 +786,187 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -748,4 +974,445 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60920FF1-84A9-4B15-8351-05135D19DC38}">
+  <dimension ref="A1:A43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="64" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C254B6BB-8D20-40DE-AD21-17B21D369280}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CCED7B-C944-4DAF-A3BE-38195A716237}">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E79526-C442-483C-B085-96826ED95061}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor stanislaus json file
</commit_message>
<xml_diff>
--- a/preprocessing/USGS Gauge Flow Data extraction/USGS gauges.xlsx
+++ b/preprocessing/USGS Gauge Flow Data extraction/USGS gauges.xlsx
@@ -8,30 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\PROJECTS\SIERRA2\Pywr models\preprocessing\USGS Gauge Flow Data extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11F6287-916A-49FB-ABD1-935C5BB02F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD4C9F0-1A75-43DA-A330-983D7DA3BC57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merced - streamflow" sheetId="1" r:id="rId1"/>
     <sheet name="merced - storage" sheetId="3" r:id="rId2"/>
-    <sheet name="stanislaus" sheetId="2" r:id="rId3"/>
-    <sheet name="upper san joaquin - streamflow" sheetId="4" r:id="rId4"/>
-    <sheet name="upper san joaquin - storage" sheetId="5" r:id="rId5"/>
-    <sheet name="tuolumne - streamflow" sheetId="6" r:id="rId6"/>
-    <sheet name="tuolumne - storage" sheetId="7" r:id="rId7"/>
+    <sheet name="stanislaus - streamflow" sheetId="2" r:id="rId3"/>
+    <sheet name="stanislaus - storage" sheetId="8" r:id="rId4"/>
+    <sheet name="upper san joaquin - streamflow" sheetId="4" r:id="rId5"/>
+    <sheet name="upper san joaquin - storage" sheetId="5" r:id="rId6"/>
+    <sheet name="tuolumne - streamflow" sheetId="6" r:id="rId7"/>
+    <sheet name="tuolumne - storage" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>USGS 11264500 MERCED R A HAPPY ISLES BRIDGE NR YOSEMITE CA</t>
   </si>
@@ -394,6 +403,36 @@
   </si>
   <si>
     <t>USGS 11249500 MADERA CN A FRIANT CA</t>
+  </si>
+  <si>
+    <t>USGS 11293370 UTICA RES NR BIG MEADOWS CA</t>
+  </si>
+  <si>
+    <t>USGS 11293350 UNION RES NR BIG MEADOWS CA</t>
+  </si>
+  <si>
+    <t>USGS 11293770 NEW SPICER MEADOW RES NR BIG MEADOW CA</t>
+  </si>
+  <si>
+    <t>USGS 11292600 DONNELL LK NR DARDANELLE CA</t>
+  </si>
+  <si>
+    <t>USGS 11291000 RELIEF RES NR BAKER STATION CA</t>
+  </si>
+  <si>
+    <t>USGS 11292800 BEARDSLEY LAKE NEAR STRAWBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11297700 LYONS RES NR LONG BARN CA</t>
+  </si>
+  <si>
+    <t>USGS 11299000 NEW MELONES RES NR SONORA CA</t>
+  </si>
+  <si>
+    <t>USGS 11295900 PINECREST LK NR STRAWBERRY CA</t>
+  </si>
+  <si>
+    <t>USGS 11299995 TULLOCH RES NR KNIGHTS FERRY CA</t>
   </si>
 </sst>
 </file>
@@ -792,12 +831,12 @@
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -986,10 +1025,79 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AEE754-2BE5-4781-AA16-1F6A506BBE5E}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A10">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60920FF1-84A9-4B15-8351-05135D19DC38}">
   <dimension ref="A1:A46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
@@ -1237,7 +1345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C254B6BB-8D20-40DE-AD21-17B21D369280}">
   <dimension ref="A1:A9"/>
   <sheetViews>
@@ -1301,7 +1409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CCED7B-C944-4DAF-A3BE-38195A716237}">
   <dimension ref="A1:A18"/>
   <sheetViews>
@@ -1409,7 +1517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E79526-C442-483C-B085-96826ED95061}">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>